<commit_message>
coverages and quote and forms updated
</commit_message>
<xml_diff>
--- a/testdata/PC_PersonalAuto.xlsx
+++ b/testdata/PC_PersonalAuto.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labor\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A9408F-C1E7-4B24-B3D7-60FE8380531B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{50BBEFF5-2ECA-4EB9-82E0-A18C62C03F9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19740" windowHeight="10965" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="8" r:id="rId1"/>
@@ -25,13 +20,16 @@
     <sheet name="drivers" sheetId="18" r:id="rId10"/>
     <sheet name="vehicles" sheetId="19" r:id="rId11"/>
     <sheet name="paCoverages" sheetId="10" r:id="rId12"/>
-    <sheet name="riskAnalysis" sheetId="14" r:id="rId13"/>
-    <sheet name="policyReview" sheetId="15" r:id="rId14"/>
-    <sheet name="forms" sheetId="17" r:id="rId15"/>
-    <sheet name="payments" sheetId="16" r:id="rId16"/>
-    <sheet name="AcctSummary" sheetId="5" r:id="rId17"/>
+    <sheet name="paQuote" sheetId="20" r:id="rId13"/>
+    <sheet name="paForms" sheetId="21" r:id="rId14"/>
+    <sheet name="riskAnalysis" sheetId="14" r:id="rId15"/>
+    <sheet name="policyReview" sheetId="15" r:id="rId16"/>
+    <sheet name="forms" sheetId="17" r:id="rId17"/>
+    <sheet name="payments" sheetId="16" r:id="rId18"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="405">
   <si>
     <t>TD_UserName</t>
   </si>
@@ -1199,13 +1197,73 @@
   </si>
   <si>
     <t>Test request approval</t>
+  </si>
+  <si>
+    <t>MedicalLimit</t>
+  </si>
+  <si>
+    <t>UnderinsuredMotoristPropertyDamageLimit</t>
+  </si>
+  <si>
+    <t>RentalCarLossofUseLimit</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>AUT_PC_AC_05</t>
+  </si>
+  <si>
+    <t>PA 00DS</t>
+  </si>
+  <si>
+    <t>Dec Sheet</t>
+  </si>
+  <si>
+    <t>AUT_PC_AC_06</t>
+  </si>
+  <si>
+    <t>ModelYear</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>refer#creatAccount</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>refer#vehicles</t>
+  </si>
+  <si>
+    <t>ComprehensiveCoverage</t>
+  </si>
+  <si>
+    <t>CollisionCoverage</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,6 +1286,24 @@
     <font>
       <sz val="11"/>
       <color rgb="FF545C67"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
@@ -1279,7 +1355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1336,6 +1412,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3263,36 +3351,62 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB72CC37-2FC1-4BE3-AA8A-0E623FF584F9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>391</v>
+      </c>
       <c r="B2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>276</v>
-      </c>
-    </row>
+      <c r="C2" s="23">
+        <v>5000</v>
+      </c>
+      <c r="D2" s="25">
+        <v>25000</v>
+      </c>
+      <c r="E2" s="27">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3312,6 +3426,136 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1401A1-3A94-45DB-A398-FF2CB40F0382}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H1" t="s">
+        <v>401</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="E2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="H2" s="30">
+        <v>7</v>
+      </c>
+      <c r="I2" s="31">
+        <v>11</v>
+      </c>
+      <c r="J2" s="33">
+        <v>713</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE31411-9014-4013-BE48-8F22F3B0F254}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1207CFE-F119-4177-89B2-C0F6EDB7E96C}">
   <dimension ref="A1:W3"/>
   <sheetViews>
@@ -3486,7 +3730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB19428-F55B-4DA0-BE94-1CF59EA9DC1E}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
@@ -3779,7 +4023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B2C3DE-BF0D-4F16-B400-5AB4FAB055AF}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3791,7 +4035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5823DF25-AE77-45CF-B610-BFA5969792F1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3805,11 +4049,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Account creation executions done
</commit_message>
<xml_diff>
--- a/testdata/PC_PersonalAuto.xlsx
+++ b/testdata/PC_PersonalAuto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labor\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C798CF8-4A53-43D8-B898-AD111EA6E209}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD38381-538E-4CA1-B925-06AF30B477B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB Config" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4048" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4103" uniqueCount="613">
   <si>
     <t>su</t>
   </si>
@@ -2055,7 +2055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2194,6 +2194,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3665,17 +3669,17 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5361,7 +5365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5C4A9D-BD01-420A-BFDB-72E36C75E940}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F3" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -13878,8 +13882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
   <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13901,10 +13905,10 @@
     <col min="15" max="15" width="12.5703125" style="58" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.5703125" style="58" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="63" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" style="63" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="58" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.7109375" style="58" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" style="58" bestFit="1" customWidth="1"/>
@@ -13996,16 +14000,16 @@
       <c r="Q1" s="48" t="s">
         <v>506</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="62" t="s">
         <v>518</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="62" t="s">
         <v>517</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="62" t="s">
         <v>515</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="62" t="s">
         <v>519</v>
       </c>
       <c r="V1" s="48" t="s">
@@ -14072,12 +14076,18 @@
       <c r="Q2" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19" t="s">
+      <c r="R2" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S2" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T2" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U2" s="19"/>
+      <c r="U2" s="62">
+        <v>99501</v>
+      </c>
       <c r="V2" s="19" t="s">
         <v>556</v>
       </c>
@@ -14156,12 +14166,18 @@
       <c r="Q3" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19" t="s">
+      <c r="R3" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S3" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T3" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U3" s="19"/>
+      <c r="U3" s="62">
+        <v>99501</v>
+      </c>
       <c r="V3" s="19" t="s">
         <v>237</v>
       </c>
@@ -14230,12 +14246,18 @@
       <c r="Q4" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19" t="s">
+      <c r="R4" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S4" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T4" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U4" s="19"/>
+      <c r="U4" s="62">
+        <v>99501</v>
+      </c>
       <c r="V4" s="19" t="s">
         <v>237</v>
       </c>
@@ -14304,12 +14326,18 @@
       <c r="Q5" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19" t="s">
+      <c r="R5" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S5" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T5" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U5" s="19"/>
+      <c r="U5" s="62">
+        <v>99501</v>
+      </c>
       <c r="V5" s="19" t="s">
         <v>237</v>
       </c>
@@ -14378,12 +14406,18 @@
       <c r="Q6" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19" t="s">
+      <c r="R6" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S6" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T6" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U6" s="19"/>
+      <c r="U6" s="62">
+        <v>99501</v>
+      </c>
       <c r="V6" s="19" t="s">
         <v>237</v>
       </c>
@@ -14452,12 +14486,18 @@
       <c r="Q7" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19" t="s">
+      <c r="R7" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S7" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T7" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U7" s="19"/>
+      <c r="U7" s="62">
+        <v>99501</v>
+      </c>
       <c r="V7" s="19" t="s">
         <v>237</v>
       </c>
@@ -14526,12 +14566,18 @@
       <c r="Q8" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19" t="s">
+      <c r="R8" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S8" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T8" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U8" s="19"/>
+      <c r="U8" s="62">
+        <v>99501</v>
+      </c>
       <c r="V8" s="19" t="s">
         <v>237</v>
       </c>
@@ -14600,12 +14646,18 @@
       <c r="Q9" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19" t="s">
+      <c r="R9" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S9" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T9" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U9" s="19"/>
+      <c r="U9" s="62">
+        <v>99501</v>
+      </c>
       <c r="V9" s="19" t="s">
         <v>237</v>
       </c>
@@ -14674,12 +14726,18 @@
       <c r="Q10" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19" t="s">
+      <c r="R10" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S10" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T10" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U10" s="19"/>
+      <c r="U10" s="62">
+        <v>99501</v>
+      </c>
       <c r="V10" s="19" t="s">
         <v>237</v>
       </c>
@@ -14748,12 +14806,18 @@
       <c r="Q11" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19" t="s">
+      <c r="R11" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S11" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T11" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U11" s="19"/>
+      <c r="U11" s="62">
+        <v>99501</v>
+      </c>
       <c r="V11" s="19" t="s">
         <v>237</v>
       </c>
@@ -14822,12 +14886,18 @@
       <c r="Q12" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19" t="s">
+      <c r="R12" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S12" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T12" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U12" s="19"/>
+      <c r="U12" s="62">
+        <v>99501</v>
+      </c>
       <c r="V12" s="19" t="s">
         <v>237</v>
       </c>
@@ -14896,12 +14966,18 @@
       <c r="Q13" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19" t="s">
+      <c r="R13" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S13" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T13" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U13" s="19"/>
+      <c r="U13" s="62">
+        <v>99501</v>
+      </c>
       <c r="V13" s="19" t="s">
         <v>237</v>
       </c>
@@ -14970,12 +15046,18 @@
       <c r="Q14" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19" t="s">
+      <c r="R14" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S14" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T14" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U14" s="19"/>
+      <c r="U14" s="62">
+        <v>99501</v>
+      </c>
       <c r="V14" s="19" t="s">
         <v>237</v>
       </c>
@@ -15044,12 +15126,18 @@
       <c r="Q15" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19" t="s">
+      <c r="R15" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S15" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T15" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U15" s="19"/>
+      <c r="U15" s="62">
+        <v>99501</v>
+      </c>
       <c r="V15" s="19" t="s">
         <v>237</v>
       </c>
@@ -15118,12 +15206,18 @@
       <c r="Q16" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19" t="s">
+      <c r="R16" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S16" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T16" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U16" s="19"/>
+      <c r="U16" s="62">
+        <v>99501</v>
+      </c>
       <c r="V16" s="19" t="s">
         <v>237</v>
       </c>
@@ -15192,12 +15286,18 @@
       <c r="Q17" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19" t="s">
+      <c r="R17" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S17" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T17" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U17" s="19"/>
+      <c r="U17" s="62">
+        <v>99501</v>
+      </c>
       <c r="V17" s="19" t="s">
         <v>237</v>
       </c>
@@ -15266,12 +15366,18 @@
       <c r="Q18" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19" t="s">
+      <c r="R18" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S18" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T18" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U18" s="19"/>
+      <c r="U18" s="62">
+        <v>99501</v>
+      </c>
       <c r="V18" s="19" t="s">
         <v>237</v>
       </c>
@@ -15340,12 +15446,18 @@
       <c r="Q19" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19" t="s">
+      <c r="R19" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S19" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T19" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U19" s="19"/>
+      <c r="U19" s="62">
+        <v>99501</v>
+      </c>
       <c r="V19" s="19" t="s">
         <v>237</v>
       </c>
@@ -15414,12 +15526,18 @@
       <c r="Q20" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19" t="s">
+      <c r="R20" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S20" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T20" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U20" s="19"/>
+      <c r="U20" s="62">
+        <v>99501</v>
+      </c>
       <c r="V20" s="19" t="s">
         <v>237</v>
       </c>
@@ -15488,12 +15606,18 @@
       <c r="Q21" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19" t="s">
+      <c r="R21" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S21" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T21" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U21" s="19"/>
+      <c r="U21" s="62">
+        <v>99501</v>
+      </c>
       <c r="V21" s="19" t="s">
         <v>237</v>
       </c>
@@ -15562,12 +15686,18 @@
       <c r="Q22" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19" t="s">
+      <c r="R22" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S22" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T22" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U22" s="19"/>
+      <c r="U22" s="62">
+        <v>99501</v>
+      </c>
       <c r="V22" s="19" t="s">
         <v>237</v>
       </c>
@@ -15636,12 +15766,18 @@
       <c r="Q23" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19" t="s">
+      <c r="R23" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S23" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T23" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U23" s="19"/>
+      <c r="U23" s="62">
+        <v>99501</v>
+      </c>
       <c r="V23" s="19" t="s">
         <v>237</v>
       </c>
@@ -15710,12 +15846,18 @@
       <c r="Q24" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19" t="s">
+      <c r="R24" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S24" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T24" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U24" s="19"/>
+      <c r="U24" s="62">
+        <v>99501</v>
+      </c>
       <c r="V24" s="19" t="s">
         <v>237</v>
       </c>
@@ -15784,12 +15926,18 @@
       <c r="Q25" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19" t="s">
+      <c r="R25" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S25" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T25" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U25" s="19"/>
+      <c r="U25" s="62">
+        <v>99501</v>
+      </c>
       <c r="V25" s="19" t="s">
         <v>237</v>
       </c>
@@ -15858,12 +16006,18 @@
       <c r="Q26" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19" t="s">
+      <c r="R26" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S26" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T26" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U26" s="19"/>
+      <c r="U26" s="62">
+        <v>99501</v>
+      </c>
       <c r="V26" s="19" t="s">
         <v>237</v>
       </c>
@@ -15932,12 +16086,18 @@
       <c r="Q27" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19" t="s">
+      <c r="R27" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S27" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T27" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U27" s="19"/>
+      <c r="U27" s="62">
+        <v>99501</v>
+      </c>
       <c r="V27" s="19" t="s">
         <v>237</v>
       </c>
@@ -16006,12 +16166,18 @@
       <c r="Q28" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19" t="s">
+      <c r="R28" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S28" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T28" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U28" s="19"/>
+      <c r="U28" s="62">
+        <v>99501</v>
+      </c>
       <c r="V28" s="19" t="s">
         <v>237</v>
       </c>
@@ -16080,12 +16246,18 @@
       <c r="Q29" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19" t="s">
+      <c r="R29" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S29" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T29" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U29" s="19"/>
+      <c r="U29" s="62">
+        <v>99501</v>
+      </c>
       <c r="V29" s="19" t="s">
         <v>237</v>
       </c>
@@ -16154,12 +16326,18 @@
       <c r="Q30" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19" t="s">
+      <c r="R30" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S30" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T30" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U30" s="19"/>
+      <c r="U30" s="62">
+        <v>99501</v>
+      </c>
       <c r="V30" s="19" t="s">
         <v>237</v>
       </c>
@@ -16228,12 +16406,18 @@
       <c r="Q31" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19" t="s">
+      <c r="R31" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S31" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T31" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U31" s="19"/>
+      <c r="U31" s="62">
+        <v>99501</v>
+      </c>
       <c r="V31" s="19" t="s">
         <v>237</v>
       </c>
@@ -16302,12 +16486,18 @@
       <c r="Q32" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19" t="s">
+      <c r="R32" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S32" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T32" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U32" s="19"/>
+      <c r="U32" s="62">
+        <v>99501</v>
+      </c>
       <c r="V32" s="19" t="s">
         <v>237</v>
       </c>
@@ -16376,12 +16566,18 @@
       <c r="Q33" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19" t="s">
+      <c r="R33" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S33" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T33" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U33" s="19"/>
+      <c r="U33" s="62">
+        <v>99501</v>
+      </c>
       <c r="V33" s="19" t="s">
         <v>237</v>
       </c>
@@ -16450,12 +16646,18 @@
       <c r="Q34" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19" t="s">
+      <c r="R34" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S34" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T34" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U34" s="19"/>
+      <c r="U34" s="62">
+        <v>99501</v>
+      </c>
       <c r="V34" s="19" t="s">
         <v>237</v>
       </c>
@@ -16524,12 +16726,18 @@
       <c r="Q35" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19" t="s">
+      <c r="R35" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S35" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T35" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U35" s="19"/>
+      <c r="U35" s="62">
+        <v>99501</v>
+      </c>
       <c r="V35" s="19" t="s">
         <v>237</v>
       </c>
@@ -16598,12 +16806,18 @@
       <c r="Q36" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19" t="s">
+      <c r="R36" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S36" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T36" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U36" s="19"/>
+      <c r="U36" s="62">
+        <v>99501</v>
+      </c>
       <c r="V36" s="19" t="s">
         <v>237</v>
       </c>
@@ -16672,12 +16886,18 @@
       <c r="Q37" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19" t="s">
+      <c r="R37" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S37" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T37" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U37" s="19"/>
+      <c r="U37" s="62">
+        <v>99501</v>
+      </c>
       <c r="V37" s="19" t="s">
         <v>237</v>
       </c>
@@ -16746,12 +16966,18 @@
       <c r="Q38" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19" t="s">
+      <c r="R38" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S38" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T38" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U38" s="19"/>
+      <c r="U38" s="62">
+        <v>99501</v>
+      </c>
       <c r="V38" s="19" t="s">
         <v>237</v>
       </c>
@@ -16820,12 +17046,18 @@
       <c r="Q39" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19" t="s">
+      <c r="R39" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S39" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T39" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U39" s="19"/>
+      <c r="U39" s="62">
+        <v>99501</v>
+      </c>
       <c r="V39" s="19" t="s">
         <v>237</v>
       </c>
@@ -16894,12 +17126,18 @@
       <c r="Q40" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19" t="s">
+      <c r="R40" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S40" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T40" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U40" s="19"/>
+      <c r="U40" s="62">
+        <v>99501</v>
+      </c>
       <c r="V40" s="19" t="s">
         <v>237</v>
       </c>
@@ -16968,12 +17206,18 @@
       <c r="Q41" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19" t="s">
+      <c r="R41" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S41" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T41" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U41" s="19"/>
+      <c r="U41" s="62">
+        <v>99501</v>
+      </c>
       <c r="V41" s="19" t="s">
         <v>237</v>
       </c>
@@ -17042,12 +17286,18 @@
       <c r="Q42" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19" t="s">
+      <c r="R42" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S42" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T42" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U42" s="19"/>
+      <c r="U42" s="62">
+        <v>99501</v>
+      </c>
       <c r="V42" s="19" t="s">
         <v>237</v>
       </c>
@@ -17116,12 +17366,18 @@
       <c r="Q43" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19" t="s">
+      <c r="R43" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S43" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T43" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U43" s="19"/>
+      <c r="U43" s="62">
+        <v>99501</v>
+      </c>
       <c r="V43" s="19" t="s">
         <v>237</v>
       </c>
@@ -17190,12 +17446,18 @@
       <c r="Q44" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19" t="s">
+      <c r="R44" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S44" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T44" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U44" s="19"/>
+      <c r="U44" s="62">
+        <v>99501</v>
+      </c>
       <c r="V44" s="19" t="s">
         <v>237</v>
       </c>
@@ -17264,12 +17526,18 @@
       <c r="Q45" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19" t="s">
+      <c r="R45" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S45" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T45" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U45" s="19"/>
+      <c r="U45" s="62">
+        <v>99501</v>
+      </c>
       <c r="V45" s="19" t="s">
         <v>237</v>
       </c>
@@ -17338,12 +17606,18 @@
       <c r="Q46" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19" t="s">
+      <c r="R46" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S46" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T46" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U46" s="19"/>
+      <c r="U46" s="62">
+        <v>99501</v>
+      </c>
       <c r="V46" s="19" t="s">
         <v>237</v>
       </c>
@@ -17412,12 +17686,18 @@
       <c r="Q47" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19" t="s">
+      <c r="R47" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S47" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T47" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U47" s="19"/>
+      <c r="U47" s="62">
+        <v>99501</v>
+      </c>
       <c r="V47" s="19" t="s">
         <v>237</v>
       </c>
@@ -17486,12 +17766,18 @@
       <c r="Q48" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R48" s="19"/>
-      <c r="S48" s="19"/>
-      <c r="T48" s="19" t="s">
+      <c r="R48" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S48" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T48" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U48" s="19"/>
+      <c r="U48" s="62">
+        <v>99501</v>
+      </c>
       <c r="V48" s="19" t="s">
         <v>237</v>
       </c>
@@ -17560,12 +17846,18 @@
       <c r="Q49" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R49" s="19"/>
-      <c r="S49" s="19"/>
-      <c r="T49" s="19" t="s">
+      <c r="R49" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S49" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T49" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U49" s="19"/>
+      <c r="U49" s="62">
+        <v>99501</v>
+      </c>
       <c r="V49" s="19" t="s">
         <v>237</v>
       </c>
@@ -17634,12 +17926,18 @@
       <c r="Q50" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
-      <c r="T50" s="19" t="s">
+      <c r="R50" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S50" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T50" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U50" s="19"/>
+      <c r="U50" s="62">
+        <v>99501</v>
+      </c>
       <c r="V50" s="19" t="s">
         <v>237</v>
       </c>
@@ -17708,12 +18006,18 @@
       <c r="Q51" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R51" s="19"/>
-      <c r="S51" s="19"/>
-      <c r="T51" s="19" t="s">
+      <c r="R51" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S51" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T51" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U51" s="19"/>
+      <c r="U51" s="62">
+        <v>99501</v>
+      </c>
       <c r="V51" s="19" t="s">
         <v>237</v>
       </c>
@@ -17782,12 +18086,18 @@
       <c r="Q52" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R52" s="19"/>
-      <c r="S52" s="19"/>
-      <c r="T52" s="19" t="s">
+      <c r="R52" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S52" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T52" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U52" s="19"/>
+      <c r="U52" s="62">
+        <v>99501</v>
+      </c>
       <c r="V52" s="19" t="s">
         <v>237</v>
       </c>
@@ -17856,12 +18166,18 @@
       <c r="Q53" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R53" s="19"/>
-      <c r="S53" s="19"/>
-      <c r="T53" s="19" t="s">
+      <c r="R53" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S53" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T53" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U53" s="19"/>
+      <c r="U53" s="62">
+        <v>99501</v>
+      </c>
       <c r="V53" s="19" t="s">
         <v>237</v>
       </c>
@@ -17930,12 +18246,18 @@
       <c r="Q54" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R54" s="19"/>
-      <c r="S54" s="19"/>
-      <c r="T54" s="19" t="s">
+      <c r="R54" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S54" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T54" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U54" s="19"/>
+      <c r="U54" s="62">
+        <v>99501</v>
+      </c>
       <c r="V54" s="19" t="s">
         <v>237</v>
       </c>
@@ -18004,12 +18326,18 @@
       <c r="Q55" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R55" s="19"/>
-      <c r="S55" s="19"/>
-      <c r="T55" s="19" t="s">
+      <c r="R55" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S55" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T55" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U55" s="19"/>
+      <c r="U55" s="62">
+        <v>99501</v>
+      </c>
       <c r="V55" s="19" t="s">
         <v>237</v>
       </c>
@@ -18078,12 +18406,18 @@
       <c r="Q56" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="R56" s="19"/>
-      <c r="S56" s="19"/>
-      <c r="T56" s="19" t="s">
+      <c r="R56" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="S56" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="T56" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="U56" s="19"/>
+      <c r="U56" s="62">
+        <v>99501</v>
+      </c>
       <c r="V56" s="19" t="s">
         <v>237</v>
       </c>
@@ -18148,8 +18482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB62B0-3E14-40DE-9CB1-C3C158CCA48E}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18228,9 +18562,7 @@
         <v>234</v>
       </c>
       <c r="E2" s="32"/>
-      <c r="F2" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F2" s="32"/>
       <c r="G2" s="32"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
@@ -18260,9 +18592,7 @@
         <v>234</v>
       </c>
       <c r="E3" s="32"/>
-      <c r="F3" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
@@ -18292,9 +18622,7 @@
         <v>234</v>
       </c>
       <c r="E4" s="32"/>
-      <c r="F4" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F4" s="32"/>
       <c r="G4" s="32"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
@@ -18324,9 +18652,7 @@
         <v>234</v>
       </c>
       <c r="E5" s="32"/>
-      <c r="F5" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F5" s="32"/>
       <c r="G5" s="32"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
@@ -18356,9 +18682,7 @@
         <v>234</v>
       </c>
       <c r="E6" s="32"/>
-      <c r="F6" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F6" s="32"/>
       <c r="G6" s="32"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
@@ -18388,9 +18712,7 @@
         <v>234</v>
       </c>
       <c r="E7" s="32"/>
-      <c r="F7" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
@@ -18420,9 +18742,7 @@
         <v>234</v>
       </c>
       <c r="E8" s="32"/>
-      <c r="F8" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
@@ -18452,9 +18772,7 @@
         <v>234</v>
       </c>
       <c r="E9" s="32"/>
-      <c r="F9" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
@@ -18484,9 +18802,7 @@
         <v>234</v>
       </c>
       <c r="E10" s="32"/>
-      <c r="F10" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
@@ -18516,9 +18832,7 @@
         <v>234</v>
       </c>
       <c r="E11" s="32"/>
-      <c r="F11" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
@@ -18548,9 +18862,7 @@
         <v>234</v>
       </c>
       <c r="E12" s="32"/>
-      <c r="F12" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
@@ -18580,9 +18892,7 @@
         <v>234</v>
       </c>
       <c r="E13" s="32"/>
-      <c r="F13" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
@@ -18612,9 +18922,7 @@
         <v>234</v>
       </c>
       <c r="E14" s="32"/>
-      <c r="F14" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
@@ -18644,9 +18952,7 @@
         <v>234</v>
       </c>
       <c r="E15" s="32"/>
-      <c r="F15" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
@@ -18676,9 +18982,7 @@
         <v>234</v>
       </c>
       <c r="E16" s="32"/>
-      <c r="F16" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
@@ -18708,9 +19012,7 @@
         <v>234</v>
       </c>
       <c r="E17" s="32"/>
-      <c r="F17" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
@@ -18740,9 +19042,7 @@
         <v>234</v>
       </c>
       <c r="E18" s="32"/>
-      <c r="F18" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
@@ -18772,9 +19072,7 @@
         <v>234</v>
       </c>
       <c r="E19" s="32"/>
-      <c r="F19" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
@@ -18804,9 +19102,7 @@
         <v>234</v>
       </c>
       <c r="E20" s="32"/>
-      <c r="F20" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4" t="s">
@@ -18836,9 +19132,7 @@
         <v>234</v>
       </c>
       <c r="E21" s="32"/>
-      <c r="F21" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
@@ -18868,9 +19162,7 @@
         <v>234</v>
       </c>
       <c r="E22" s="32"/>
-      <c r="F22" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
@@ -18900,9 +19192,7 @@
         <v>234</v>
       </c>
       <c r="E23" s="32"/>
-      <c r="F23" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
@@ -18932,9 +19222,7 @@
         <v>234</v>
       </c>
       <c r="E24" s="32"/>
-      <c r="F24" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F24" s="32"/>
       <c r="G24" s="32"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
@@ -18964,9 +19252,7 @@
         <v>234</v>
       </c>
       <c r="E25" s="32"/>
-      <c r="F25" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
@@ -18996,9 +19282,7 @@
         <v>234</v>
       </c>
       <c r="E26" s="32"/>
-      <c r="F26" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
@@ -19028,9 +19312,7 @@
         <v>234</v>
       </c>
       <c r="E27" s="32"/>
-      <c r="F27" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
@@ -19060,9 +19342,7 @@
         <v>234</v>
       </c>
       <c r="E28" s="32"/>
-      <c r="F28" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F28" s="32"/>
       <c r="G28" s="32"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
@@ -19092,9 +19372,7 @@
         <v>234</v>
       </c>
       <c r="E29" s="32"/>
-      <c r="F29" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F29" s="32"/>
       <c r="G29" s="32"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
@@ -19124,9 +19402,7 @@
         <v>234</v>
       </c>
       <c r="E30" s="32"/>
-      <c r="F30" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
@@ -19156,9 +19432,7 @@
         <v>234</v>
       </c>
       <c r="E31" s="32"/>
-      <c r="F31" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F31" s="32"/>
       <c r="G31" s="32"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
@@ -19188,9 +19462,7 @@
         <v>234</v>
       </c>
       <c r="E32" s="32"/>
-      <c r="F32" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F32" s="32"/>
       <c r="G32" s="32"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
@@ -19220,9 +19492,7 @@
         <v>234</v>
       </c>
       <c r="E33" s="32"/>
-      <c r="F33" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
@@ -19252,9 +19522,7 @@
         <v>234</v>
       </c>
       <c r="E34" s="32"/>
-      <c r="F34" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
@@ -19284,9 +19552,7 @@
         <v>234</v>
       </c>
       <c r="E35" s="32"/>
-      <c r="F35" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F35" s="32"/>
       <c r="G35" s="32"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
@@ -19316,9 +19582,7 @@
         <v>234</v>
       </c>
       <c r="E36" s="32"/>
-      <c r="F36" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4" t="s">
@@ -19348,9 +19612,7 @@
         <v>234</v>
       </c>
       <c r="E37" s="32"/>
-      <c r="F37" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4" t="s">
@@ -19380,9 +19642,7 @@
         <v>234</v>
       </c>
       <c r="E38" s="32"/>
-      <c r="F38" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4" t="s">
@@ -19412,9 +19672,7 @@
         <v>234</v>
       </c>
       <c r="E39" s="32"/>
-      <c r="F39" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4" t="s">
@@ -19444,9 +19702,7 @@
         <v>234</v>
       </c>
       <c r="E40" s="32"/>
-      <c r="F40" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
@@ -19476,9 +19732,7 @@
         <v>234</v>
       </c>
       <c r="E41" s="32"/>
-      <c r="F41" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F41" s="32"/>
       <c r="G41" s="32"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4" t="s">
@@ -19508,9 +19762,7 @@
         <v>234</v>
       </c>
       <c r="E42" s="32"/>
-      <c r="F42" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F42" s="32"/>
       <c r="G42" s="32"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4" t="s">
@@ -19540,9 +19792,7 @@
         <v>234</v>
       </c>
       <c r="E43" s="32"/>
-      <c r="F43" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F43" s="32"/>
       <c r="G43" s="32"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4" t="s">
@@ -19572,9 +19822,7 @@
         <v>234</v>
       </c>
       <c r="E44" s="32"/>
-      <c r="F44" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
@@ -19604,9 +19852,7 @@
         <v>234</v>
       </c>
       <c r="E45" s="32"/>
-      <c r="F45" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4" t="s">
@@ -19636,9 +19882,7 @@
         <v>234</v>
       </c>
       <c r="E46" s="32"/>
-      <c r="F46" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
@@ -19668,9 +19912,7 @@
         <v>234</v>
       </c>
       <c r="E47" s="32"/>
-      <c r="F47" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
@@ -19700,9 +19942,7 @@
         <v>234</v>
       </c>
       <c r="E48" s="32"/>
-      <c r="F48" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F48" s="32"/>
       <c r="G48" s="32"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
@@ -19732,9 +19972,7 @@
         <v>234</v>
       </c>
       <c r="E49" s="32"/>
-      <c r="F49" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F49" s="32"/>
       <c r="G49" s="32"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4" t="s">
@@ -19764,9 +20002,7 @@
         <v>234</v>
       </c>
       <c r="E50" s="32"/>
-      <c r="F50" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F50" s="32"/>
       <c r="G50" s="32"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
@@ -19796,9 +20032,7 @@
         <v>234</v>
       </c>
       <c r="E51" s="32"/>
-      <c r="F51" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F51" s="32"/>
       <c r="G51" s="32"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
@@ -19828,9 +20062,7 @@
         <v>234</v>
       </c>
       <c r="E52" s="32"/>
-      <c r="F52" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F52" s="32"/>
       <c r="G52" s="32"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
@@ -19860,9 +20092,7 @@
         <v>234</v>
       </c>
       <c r="E53" s="32"/>
-      <c r="F53" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F53" s="32"/>
       <c r="G53" s="32"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4" t="s">
@@ -19892,9 +20122,7 @@
         <v>234</v>
       </c>
       <c r="E54" s="32"/>
-      <c r="F54" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F54" s="32"/>
       <c r="G54" s="32"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4" t="s">
@@ -19924,9 +20152,7 @@
         <v>234</v>
       </c>
       <c r="E55" s="32"/>
-      <c r="F55" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F55" s="32"/>
       <c r="G55" s="32"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
@@ -19956,9 +20182,7 @@
         <v>234</v>
       </c>
       <c r="E56" s="32"/>
-      <c r="F56" s="32" t="s">
-        <v>247</v>
-      </c>
+      <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4" t="s">
@@ -20944,8 +21168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3B6735-2BBD-431A-8627-1925B404C972}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A54"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21897,7 +22121,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>